<commit_message>
fix: feedback correction and finalise unit test
</commit_message>
<xml_diff>
--- a/test/project-config/forms/app/patient_assessment_under_5.xlsx
+++ b/test/project-config/forms/app/patient_assessment_under_5.xlsx
@@ -24738,7 +24738,7 @@
       <c r="T552" s="126"/>
       <c r="U552" s="115"/>
     </row>
-    <row r="553" ht="15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="553" ht="15" customHeight="1" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C553" s="1"/>
       <c r="D553" s="1"/>
       <c r="E553" s="1"/>
@@ -26640,10 +26640,10 @@
     <row r="617" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="618" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="619" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" ht="15" customHeight="1" spans="1:23" x14ac:dyDescent="0.25"/>
-    <row r="621" ht="15" customHeight="1" spans="1:23" x14ac:dyDescent="0.25"/>
-    <row r="622" ht="15" customHeight="1" spans="1:23" x14ac:dyDescent="0.25"/>
-    <row r="623" ht="15" customHeight="1" spans="1:23" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" sqref="A1:A90">

</xml_diff>